<commit_message>
lyla: add writeup; pick a new Chinese name
</commit_message>
<xml_diff>
--- a/lyla/docs/题目基本信息.xlsx
+++ b/lyla/docs/题目基本信息.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riatre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\src\github.com\Riatre\aliyunctf-2022-challenges\lyla\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513A8764-A572-40CD-AC1C-0BD795748B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>re-莱娜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Is this really solvable? https://en.wikipedia.org/wiki/Speck_(cipher)#:~:text=%5Bedit%5D-,Cryptanalysis,-%5Bedit%5D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,10 +80,6 @@
   </si>
   <si>
     <t>1 * ECS 2c 2g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本行为 lyla 的中文信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -103,13 +96,21 @@
     <t>面对如此传统的逆向工程题目，代码量不大，输入密码换取 flag 的经典设计，你还在等什么，快来解它！
 注意：题目保证有解，但解不唯一。
 nc &lt;ip&gt; 1337</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>re-莱拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本行为 lyla 的中文信息；题目名字没有中文含义，保留了英文，如果不行，用“利拉”这种音译</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,11 +431,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -480,16 +481,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -498,21 +499,21 @@
         <v>1337</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>